<commit_message>
feat: add Reports icon to quick access with situational report dropdown
</commit_message>
<xml_diff>
--- a/CADASTRO DE ABRIGOS.xlsx
+++ b/CADASTRO DE ABRIGOS.xlsx
@@ -8,27 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DEFESA_CIVIL_MOBILE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8050DC7-BB82-4C78-B701-CB9D64B3EE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21BBB36-6D49-4A87-B69A-64BD66E5958C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -468,7 +455,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>